<commit_message>
changing comparasion and recent ddls
</commit_message>
<xml_diff>
--- a/Live.Optics.DataDomainAutomationTests/ASUPS/APM00135225329/ Data Domain Replication Mapping - 2019-07-06.xlsx
+++ b/Live.Optics.DataDomainAutomationTests/ASUPS/APM00135225329/ Data Domain Replication Mapping - 2019-07-06.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Mtree and Dir Replication" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mtree and Dir Replication'!$A$1:$O$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mtree and Dir Replication'!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>Data Domain Serial</t>
   </si>
@@ -72,6 +72,12 @@
   <si>
     <t>Sat Jul  6 15:21</t>
   </si>
+  <si>
+    <t>APM00164300001</t>
+  </si>
+  <si>
+    <t>Sat Oct 19 15:58</t>
+  </si>
 </sst>
 </file>
 
@@ -94,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +116,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0D0D0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,13 +153,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -464,7 +479,7 @@
     <col min="12" max="12" width="28.5703125" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
     <col min="14" max="14" width="23.7109375" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -594,21 +609,51 @@
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -3861,7 +3906,7 @@
       <c r="AE101" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O3"/>
+  <autoFilter ref="A1:O4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>